<commit_message>
Upload sync data commulative
</commit_message>
<xml_diff>
--- a/data/sync_datasets.xlsx
+++ b/data/sync_datasets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\Desktop\UA\5º Carrera\Sistemas Inteligentes\hackaton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\djp10\hackaton\nasa-space-apps-challenge\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF56CEC-D0F9-4F5C-912B-10491EB5AFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8551CC29-8CA0-4B7B-87A2-93226D9A880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>#</t>
   </si>
@@ -157,19 +157,101 @@
   </si>
   <si>
     <t>TOI</t>
+  </si>
+  <si>
+    <t>Commulative</t>
+  </si>
+  <si>
+    <t>koi_period</t>
+  </si>
+  <si>
+    <t>koi_depth</t>
+  </si>
+  <si>
+    <t>koi_duration</t>
+  </si>
+  <si>
+    <t>koi_model_snr</t>
+  </si>
+  <si>
+    <t>No available</t>
+  </si>
+  <si>
+    <t>koi_fpflag_ss</t>
+  </si>
+  <si>
+    <t>koi_timeObk</t>
+  </si>
+  <si>
+    <t>koi_disposition</t>
+  </si>
+  <si>
+    <t>koi_fpflag_co</t>
+  </si>
+  <si>
+    <t>koi_kepmag</t>
+  </si>
+  <si>
+    <r>
+      <t>koi_steff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>koi_slogg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>koi_srad</t>
+    </r>
+  </si>
+  <si>
+    <t>koi_impact,koi_prad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -207,8 +289,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,46 +571,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -538,11 +620,14 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -552,11 +637,14 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3</v>
       </c>
@@ -566,11 +654,14 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -580,11 +671,14 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
@@ -594,11 +688,14 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -608,11 +705,14 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
       <c r="F8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>7</v>
       </c>
@@ -622,11 +722,14 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>8</v>
       </c>
@@ -636,11 +739,14 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>9</v>
       </c>
@@ -650,11 +756,14 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10</v>
       </c>
@@ -664,11 +773,14 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>11</v>
       </c>
@@ -678,11 +790,14 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>12</v>
       </c>
@@ -692,11 +807,14 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
       <c r="F14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>13</v>
       </c>
@@ -706,11 +824,14 @@
       <c r="D15" t="s">
         <v>37</v>
       </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>14</v>
       </c>
@@ -720,11 +841,14 @@
       <c r="D16" t="s">
         <v>38</v>
       </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>15</v>
       </c>
@@ -733,6 +857,9 @@
       </c>
       <c r="D17" t="s">
         <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>

</xml_diff>